<commit_message>
Corrección de celdas sopadeletras
</commit_message>
<xml_diff>
--- a/pausas_activas.xlsx
+++ b/pausas_activas.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
@@ -2227,6 +2227,366 @@
         <v>20</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>11639</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>EDRIAN ALONSO BENITEZ ESCOBAR</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2025-05-16T10:52</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>SELL E</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>10:55:12 a.m.</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>10:55:59 a.m.</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>11639</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>EDRIAN ALONSO BENITEZ ESCOBAR</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2025-05-16T10:56</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>SELL E</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>10:57:08 a.m.</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>10:57:09 a.m.</t>
+        </is>
+      </c>
+      <c r="H66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>11639</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>EDRIAN ALONSO BENITEZ ESCOBAR</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2025-05-20T14:32</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>SELL E</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>2:33:39 p.m.</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2:34:38 p.m.</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>11227</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>JOHANA ANDREA GONZALEZ LOPEZ</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2025-05-20T14:34</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>ADIT E</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>2:34:54 p.m.</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2:35:18 p.m.</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>11636</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>YOVANI ANDRES  BEDOYA PEREZ</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2025-05-26T14:38</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>SELL E</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>2:38:50 p.m.</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2:39:32 p.m.</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>10640</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Jhonnattan Ruiz</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2025-06-12T13:09</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>ADM E</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>1:49:02 p.m.</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>1:49:12 p.m.</t>
+        </is>
+      </c>
+      <c r="H70" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>11639</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>EDRIAN ALONSO BENITEZ ESCOBAR</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>2025-07-09T13:52</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>SELL E</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>1:52:53 p.m.</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>1:53:05 p.m.</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>11639</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>EDRIAN ALONSO BENITEZ ESCOBAR</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2025-08-05T12:55</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>SELL E</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>12:56:01 p.m.</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>12:56:40 p.m.</t>
+        </is>
+      </c>
+      <c r="H72" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>11639</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>EDRIAN ALONSO BENITEZ ESCOBAR</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>2025-08-05T13:20</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>SELL E</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>1:20:13 p.m.</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>1:22:13 p.m.</t>
+        </is>
+      </c>
+      <c r="H73" t="n">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>